<commit_message>
Import works (kind of)
</commit_message>
<xml_diff>
--- a/database/Chauffeurs.xlsx
+++ b/database/Chauffeurs.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Chauffeurs" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chauffeurs!$A$1:$D$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Chauffeurs!$A$1:$D$62</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="234">
   <si>
     <t>Nom</t>
   </si>
@@ -56,9 +56,6 @@
     <t>+41792042146</t>
   </si>
   <si>
-    <t>Angiolilli Perrin</t>
-  </si>
-  <si>
     <t>Aude</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>+41793988400</t>
   </si>
   <si>
-    <t>Féry</t>
-  </si>
-  <si>
     <t>Christine</t>
   </si>
   <si>
@@ -368,18 +362,6 @@
     <t>+41793014985</t>
   </si>
   <si>
-    <t>Glaus</t>
-  </si>
-  <si>
-    <t>Vania</t>
-  </si>
-  <si>
-    <t>vania.glaus@icloud.com</t>
-  </si>
-  <si>
-    <t>079 799 04 64</t>
-  </si>
-  <si>
     <t>Grosjean</t>
   </si>
   <si>
@@ -428,18 +410,6 @@
     <t>+41792479665</t>
   </si>
   <si>
-    <t>Janin Cancian</t>
-  </si>
-  <si>
-    <t>Léonore</t>
-  </si>
-  <si>
-    <t>leonorecancian@gmail.com</t>
-  </si>
-  <si>
-    <t>+41787971005</t>
-  </si>
-  <si>
     <t>Janin</t>
   </si>
   <si>
@@ -524,30 +494,6 @@
     <t>+41763692383</t>
   </si>
   <si>
-    <t>Mariotti</t>
-  </si>
-  <si>
-    <t>Monica</t>
-  </si>
-  <si>
-    <t>monicamariotti@romandie.com</t>
-  </si>
-  <si>
-    <t>078 735 13 19</t>
-  </si>
-  <si>
-    <t>Marquis</t>
-  </si>
-  <si>
-    <t>Marie Jo</t>
-  </si>
-  <si>
-    <t>majolo@bluewin.ch</t>
-  </si>
-  <si>
-    <t>0793949561</t>
-  </si>
-  <si>
     <t>Martin</t>
   </si>
   <si>
@@ -626,12 +572,6 @@
     <t>+41786200894</t>
   </si>
   <si>
-    <t>Pinilla Marin</t>
-  </si>
-  <si>
-    <t>Andres Ricardo</t>
-  </si>
-  <si>
     <t>andres.pinillamarin@hotmail.com</t>
   </si>
   <si>
@@ -662,18 +602,6 @@
     <t>076 369 19 14</t>
   </si>
   <si>
-    <t>Ramella</t>
-  </si>
-  <si>
-    <t>Elodie</t>
-  </si>
-  <si>
-    <t>elodie.ramella@gmail.com</t>
-  </si>
-  <si>
-    <t>0792186113</t>
-  </si>
-  <si>
     <t>Ramos</t>
   </si>
   <si>
@@ -789,6 +717,21 @@
   </si>
   <si>
     <t>+41786966890</t>
+  </si>
+  <si>
+    <t>Féry-Hammer</t>
+  </si>
+  <si>
+    <t>Fleischman</t>
+  </si>
+  <si>
+    <t>Andres</t>
+  </si>
+  <si>
+    <t>Pinilla-Marin</t>
+  </si>
+  <si>
+    <t>Angiolili</t>
   </si>
 </sst>
 </file>
@@ -1228,10 +1171,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="D72" sqref="D72:D73"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1276,34 +1219,34 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F66" si="0">"UPDATE users SET email='" &amp;C3 &amp; "', phone_number='" &amp; D3 &amp; "' WHERE UPPER(firstname) = '" &amp; UPPER(B3) &amp; "' AND UPPER(lastname) = '" &amp; UPPER(A3) &amp; "';"</f>
-        <v>UPDATE users SET email='aude.angiolilli@yahoo.fr', phone_number='+41766163849' WHERE UPPER(firstname) = 'AUDE' AND UPPER(lastname) = 'ANGIOLILLI PERRIN';</v>
+        <f t="shared" ref="F3:F61" si="0">"UPDATE users SET email='" &amp;C3 &amp; "', phone_number='" &amp; D3 &amp; "' WHERE UPPER(firstname) = '" &amp; UPPER(B3) &amp; "' AND UPPER(lastname) = '" &amp; UPPER(A3) &amp; "';"</f>
+        <v>UPDATE users SET email='aude.angiolilli@yahoo.fr', phone_number='+41766163849' WHERE UPPER(firstname) = 'AUDE' AND UPPER(lastname) = 'ANGIOLILI';</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
@@ -1312,16 +1255,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="D5" t="s">
-        <v>19</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
@@ -1330,16 +1273,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
@@ -1348,16 +1291,16 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="D7" t="s">
-        <v>27</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
@@ -1366,16 +1309,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>30</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
@@ -1384,16 +1327,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>35</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
@@ -1402,16 +1345,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>39</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
@@ -1420,16 +1363,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
@@ -1438,16 +1381,16 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
         <v>44</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
@@ -1456,16 +1399,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
@@ -1474,16 +1417,16 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>54</v>
-      </c>
-      <c r="D14" t="s">
-        <v>55</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
@@ -1492,16 +1435,16 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>58</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
@@ -1510,16 +1453,16 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>61</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>62</v>
-      </c>
-      <c r="D16" t="s">
-        <v>63</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -1528,16 +1471,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
+        <v>63</v>
+      </c>
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>65</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>66</v>
-      </c>
-      <c r="D17" t="s">
-        <v>67</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
@@ -1546,16 +1489,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>70</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
@@ -1564,16 +1507,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
       <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="s">
         <v>73</v>
-      </c>
-      <c r="D19" t="s">
-        <v>74</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
@@ -1582,34 +1525,34 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
         <v>76</v>
       </c>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='christine.fery-hammer@hesge.ch', phone_number='+41797564981' WHERE UPPER(firstname) = 'CHRISTINE' AND UPPER(lastname) = 'FÉRY';</v>
+        <v>UPDATE users SET email='christine.fery-hammer@hesge.ch', phone_number='+41797564981' WHERE UPPER(firstname) = 'CHRISTINE' AND UPPER(lastname) = 'FÉRY-HAMMER';</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
         <v>79</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
@@ -1618,34 +1561,34 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>230</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
         <v>82</v>
       </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='rofl62@gmail.com', phone_number='+41792068823' WHERE UPPER(firstname) = 'ROLAND' AND UPPER(lastname) = 'FLEISCHMANN';</v>
+        <v>UPDATE users SET email='rofl62@gmail.com', phone_number='+41792068823' WHERE UPPER(firstname) = 'ROLAND' AND UPPER(lastname) = 'FLEISCHMAN';</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
         <v>85</v>
       </c>
-      <c r="B23" t="s">
+      <c r="D23" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
@@ -1654,16 +1597,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
         <v>89</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
@@ -1672,16 +1615,16 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
         <v>93</v>
       </c>
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
@@ -1690,16 +1633,16 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
+        <v>95</v>
+      </c>
+      <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
         <v>97</v>
       </c>
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
@@ -1708,16 +1651,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" t="s">
         <v>101</v>
-      </c>
-      <c r="C27" t="s">
-        <v>102</v>
-      </c>
-      <c r="D27" t="s">
-        <v>103</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
@@ -1726,16 +1669,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" t="s">
         <v>104</v>
       </c>
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>105</v>
-      </c>
-      <c r="C28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D28" t="s">
-        <v>107</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
@@ -1744,16 +1687,16 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
         <v>108</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>109</v>
-      </c>
-      <c r="C29" t="s">
-        <v>110</v>
-      </c>
-      <c r="D29" t="s">
-        <v>111</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
@@ -1762,690 +1705,600 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" t="s">
         <v>112</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>113</v>
       </c>
-      <c r="C30" t="s">
-        <v>114</v>
-      </c>
-      <c r="D30" t="s">
-        <v>115</v>
-      </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='vania.glaus@icloud.com', phone_number='079 799 04 64' WHERE UPPER(firstname) = 'VANIA' AND UPPER(lastname) = 'GLAUS';</v>
+        <v>UPDATE users SET email='daniel.grosjean@me.com', phone_number='+41798748363' WHERE UPPER(firstname) = 'DANIEL' AND UPPER(lastname) = 'GROSJEAN';</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
         <v>116</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>117</v>
       </c>
-      <c r="C31" t="s">
-        <v>118</v>
-      </c>
-      <c r="D31" t="s">
-        <v>119</v>
-      </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='daniel.grosjean@me.com', phone_number='+41798748363' WHERE UPPER(firstname) = 'DANIEL' AND UPPER(lastname) = 'GROSJEAN';</v>
+        <v>UPDATE users SET email='harbdavid0463@gmail.com', phone_number='0799415106' WHERE UPPER(firstname) = 'DAVID' AND UPPER(lastname) = 'HARB';</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
         <v>120</v>
       </c>
-      <c r="B32" t="s">
+      <c r="D32" t="s">
         <v>121</v>
       </c>
-      <c r="C32" t="s">
-        <v>122</v>
-      </c>
-      <c r="D32" t="s">
-        <v>123</v>
-      </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='harbdavid0463@gmail.com', phone_number='0799415106' WHERE UPPER(firstname) = 'DAVID' AND UPPER(lastname) = 'HARB';</v>
+        <v>UPDATE users SET email='k.howells@cbts.ch', phone_number='+41793486487' WHERE UPPER(firstname) = 'KEVIN' AND UPPER(lastname) = 'HOWELLS';</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" t="s">
         <v>124</v>
       </c>
-      <c r="B33" t="s">
+      <c r="D33" t="s">
         <v>125</v>
       </c>
-      <c r="C33" t="s">
-        <v>126</v>
-      </c>
-      <c r="D33" t="s">
-        <v>127</v>
-      </c>
       <c r="F33" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='k.howells@cbts.ch', phone_number='+41793486487' WHERE UPPER(firstname) = 'KEVIN' AND UPPER(lastname) = 'HOWELLS';</v>
+        <v>UPDATE users SET email='marieh12@bluewin.ch', phone_number='+41792479665' WHERE UPPER(firstname) = 'MARIE-HÉLÈNE' AND UPPER(lastname) = 'IMFELD';</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
+        <v>127</v>
+      </c>
+      <c r="C34" t="s">
         <v>128</v>
       </c>
-      <c r="B34" t="s">
+      <c r="D34" t="s">
         <v>129</v>
       </c>
-      <c r="C34" t="s">
-        <v>130</v>
-      </c>
-      <c r="D34" t="s">
-        <v>131</v>
-      </c>
       <c r="F34" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='marieh12@bluewin.ch', phone_number='+41792479665' WHERE UPPER(firstname) = 'MARIE-HÉLÈNE' AND UPPER(lastname) = 'IMFELD';</v>
+        <v>UPDATE users SET email='heloise.janin@hotmail.com', phone_number='+41788603348' WHERE UPPER(firstname) = 'HÉLOÏSE' AND UPPER(lastname) = 'JANIN';</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" t="s">
         <v>132</v>
       </c>
-      <c r="B35" t="s">
+      <c r="D35" t="s">
         <v>133</v>
       </c>
-      <c r="C35" t="s">
-        <v>134</v>
-      </c>
-      <c r="D35" t="s">
-        <v>135</v>
-      </c>
       <c r="F35" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='leonorecancian@gmail.com', phone_number='+41787971005' WHERE UPPER(firstname) = 'LÉONORE' AND UPPER(lastname) = 'JANIN CANCIAN';</v>
+        <v>UPDATE users SET email='leandro.jardim@hotmail.com', phone_number='+41787077253' WHERE UPPER(firstname) = 'LEANDRO' AND UPPER(lastname) = 'JARDIM';</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
+        <v>134</v>
+      </c>
+      <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
         <v>136</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
         <v>137</v>
       </c>
-      <c r="C36" t="s">
-        <v>138</v>
-      </c>
-      <c r="D36" t="s">
-        <v>139</v>
-      </c>
       <c r="F36" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='heloise.janin@hotmail.com', phone_number='+41788603348' WHERE UPPER(firstname) = 'HÉLOÏSE' AND UPPER(lastname) = 'JANIN';</v>
+        <v>UPDATE users SET email='laurentjung@bluewin.ch', phone_number='+41766162174' WHERE UPPER(firstname) = 'LAURENT' AND UPPER(lastname) = 'JUNG';</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>139</v>
+      </c>
+      <c r="D37" t="s">
         <v>140</v>
       </c>
-      <c r="B37" t="s">
-        <v>141</v>
-      </c>
-      <c r="C37" t="s">
-        <v>142</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
       <c r="F37" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='leandro.jardim@hotmail.com', phone_number='+41787077253' WHERE UPPER(firstname) = 'LEANDRO' AND UPPER(lastname) = 'JARDIM';</v>
+        <v>UPDATE users SET email='draks@sunrise.ch', phone_number='+41763406034' WHERE UPPER(firstname) = 'DAVID' AND UPPER(lastname) = 'KORKIA';</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>60</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='laurentjung@bluewin.ch', phone_number='+41766162174' WHERE UPPER(firstname) = 'LAURENT' AND UPPER(lastname) = 'JUNG';</v>
+        <v>UPDATE users SET email='pascal_kuenzi@bluewin.ch', phone_number='+41787798081' WHERE UPPER(firstname) = 'PASCAL' AND UPPER(lastname) = 'KUENZI';</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>145</v>
       </c>
       <c r="C39" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D39" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='draks@sunrise.ch', phone_number='+41763406034' WHERE UPPER(firstname) = 'DAVID' AND UPPER(lastname) = 'KORKIA';</v>
+        <v>UPDATE users SET email='elodie.lager@wanadoo.fr', phone_number='0787638728' WHERE UPPER(firstname) = 'MICHEL' AND UPPER(lastname) = 'LAGER';</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A40" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='pascal_kuenzi@bluewin.ch', phone_number='+41787798081' WHERE UPPER(firstname) = 'PASCAL' AND UPPER(lastname) = 'KUENZI';</v>
+        <v>UPDATE users SET email='bllaurent@hotmail.com', phone_number='+41786286234' WHERE UPPER(firstname) = 'BLAISE' AND UPPER(lastname) = 'LAURENT';</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>32</v>
       </c>
       <c r="C41" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D41" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F41" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='elodie.lager@wanadoo.fr', phone_number='0787638728' WHERE UPPER(firstname) = 'MICHEL' AND UPPER(lastname) = 'LAGER';</v>
+        <v>UPDATE users SET email='vincentlopez2@orange.fr', phone_number='+41763692383' WHERE UPPER(firstname) = 'VINCENT' AND UPPER(lastname) = 'LOPEZ';</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A42" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C42" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="D42" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="F42" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='bllaurent@hotmail.com', phone_number='+41786286234' WHERE UPPER(firstname) = 'BLAISE' AND UPPER(lastname) = 'LAURENT';</v>
+        <v>UPDATE users SET email='patrick.martin@cardok.com', phone_number='+41793963094' WHERE UPPER(firstname) = 'PATRICK' AND UPPER(lastname) = 'MARTIN';</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A43" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B43" t="s">
-        <v>33</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D43" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="F43" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='vincentlopez2@orange.fr', phone_number='+41763692383' WHERE UPPER(firstname) = 'VINCENT' AND UPPER(lastname) = 'LOPEZ';</v>
+        <v>UPDATE users SET email='nicoulala@yahoo.fr', phone_number='+41794617508' WHERE UPPER(firstname) = 'NICOLAS' AND UPPER(lastname) = 'MIESEGAES';</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A44" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B44" t="s">
-        <v>165</v>
+        <v>135</v>
       </c>
       <c r="C44" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D44" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F44" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='monicamariotti@romandie.com', phone_number='078 735 13 19' WHERE UPPER(firstname) = 'MONICA' AND UPPER(lastname) = 'MARIOTTI';</v>
+        <v>UPDATE users SET email='lmingard@bluewin.ch', phone_number='+41794710779' WHERE UPPER(firstname) = 'LAURENT' AND UPPER(lastname) = 'MINGARD';</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A45" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F45" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='majolo@bluewin.ch', phone_number='0793949561' WHERE UPPER(firstname) = 'MARIE JO' AND UPPER(lastname) = 'MARQUIS';</v>
+        <v>UPDATE users SET email='simone_muller@hotmail.com', phone_number='+41792398060' WHERE UPPER(firstname) = 'SIMONE' AND UPPER(lastname) = 'MULLER';</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A46" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B46" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C46" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D46" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F46" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='patrick.martin@cardok.com', phone_number='+41793963094' WHERE UPPER(firstname) = 'PATRICK' AND UPPER(lastname) = 'MARTIN';</v>
+        <v>UPDATE users SET email='perret.valerie@gmail.com', phone_number='+41793376040' WHERE UPPER(firstname) = 'VALÉRIE' AND UPPER(lastname) = 'PERRET';</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A47" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B47" t="s">
-        <v>69</v>
+        <v>173</v>
       </c>
       <c r="C47" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D47" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F47" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='nicoulala@yahoo.fr', phone_number='+41794617508' WHERE UPPER(firstname) = 'NICOLAS' AND UPPER(lastname) = 'MIESEGAES';</v>
+        <v>UPDATE users SET email='floriane.piguet@gmx.ch', phone_number='+41786206160' WHERE UPPER(firstname) = 'FLORIANE' AND UPPER(lastname) = 'PIGUET';</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" t="s">
         <v>179</v>
       </c>
-      <c r="B48" t="s">
-        <v>145</v>
-      </c>
-      <c r="C48" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" t="s">
-        <v>181</v>
-      </c>
       <c r="F48" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='lmingard@bluewin.ch', phone_number='+41794710779' WHERE UPPER(firstname) = 'LAURENT' AND UPPER(lastname) = 'MINGARD';</v>
+        <v>UPDATE users SET email='cpinillamarin@gmail.com', phone_number='+41786200894' WHERE UPPER(firstname) = 'CHRISTIAN' AND UPPER(lastname) = 'PINILLA';</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>182</v>
+        <v>232</v>
       </c>
       <c r="B49" t="s">
-        <v>183</v>
+        <v>231</v>
       </c>
       <c r="C49" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D49" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F49" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='simone_muller@hotmail.com', phone_number='+41792398060' WHERE UPPER(firstname) = 'SIMONE' AND UPPER(lastname) = 'MULLER';</v>
+        <v>UPDATE users SET email='andres.pinillamarin@hotmail.com', phone_number='+41791362132' WHERE UPPER(firstname) = 'ANDRES' AND UPPER(lastname) = 'PINILLA-MARIN';</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B50" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D50" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F50" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='perret.valerie@gmail.com', phone_number='+41793376040' WHERE UPPER(firstname) = 'VALÉRIE' AND UPPER(lastname) = 'PERRET';</v>
+        <v>UPDATE users SET email='bertrand.pouilly@ecolint.ch', phone_number='+33673139277' WHERE UPPER(firstname) = 'BERTRAND' AND UPPER(lastname) = 'POUILLY';</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A51" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B51" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="C51" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D51" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F51" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='floriane.piguet@gmx.ch', phone_number='+41786206160' WHERE UPPER(firstname) = 'FLORIANE' AND UPPER(lastname) = 'PIGUET';</v>
+        <v>UPDATE users SET email='sebastien.rais@netplus.ch', phone_number='076 369 19 14' WHERE UPPER(firstname) = 'SÉBASTIEN' AND UPPER(lastname) = 'RAIS';</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="C52" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D52" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='cpinillamarin@gmail.com', phone_number='+41786200894' WHERE UPPER(firstname) = 'CHRISTIAN' AND UPPER(lastname) = 'PINILLA';</v>
+        <v>UPDATE users SET email='joaosomar13@gmail.com', phone_number='+41766936814' WHERE UPPER(firstname) = 'JOAO' AND UPPER(lastname) = 'RAMOS';</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A53" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B53" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="C53" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D53" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='andres.pinillamarin@hotmail.com', phone_number='+41791362132' WHERE UPPER(firstname) = 'ANDRES RICARDO' AND UPPER(lastname) = 'PINILLA MARIN';</v>
+        <v>UPDATE users SET email='martine_robyr@hotmail.com', phone_number='+41765687392' WHERE UPPER(firstname) = 'MARTINE' AND UPPER(lastname) = 'ROBYR';</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A54" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B54" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C54" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="D54" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='bertrand.pouilly@ecolint.ch', phone_number='+33673139277' WHERE UPPER(firstname) = 'BERTRAND' AND UPPER(lastname) = 'POUILLY';</v>
+        <v>UPDATE users SET email='robyrs@bluewin.ch', phone_number='+41794248620' WHERE UPPER(firstname) = 'STÉPHANIE' AND UPPER(lastname) = 'ROBYR';</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A55" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B55" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C55" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D55" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='sebastien.rais@netplus.ch', phone_number='076 369 19 14' WHERE UPPER(firstname) = 'SÉBASTIEN' AND UPPER(lastname) = 'RAIS';</v>
+        <v>UPDATE users SET email='troch@windowslive.com', phone_number='+41796587802' WHERE UPPER(firstname) = 'THIERRY' AND UPPER(lastname) = 'ROCH';</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B56" t="s">
-        <v>211</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="D56" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='elodie.ramella@gmail.com', phone_number='0792186113' WHERE UPPER(firstname) = 'ELODIE' AND UPPER(lastname) = 'RAMELLA';</v>
+        <v>UPDATE users SET email='marcrosso@hotmail.com', phone_number='+41786770997' WHERE UPPER(firstname) = 'MARC' AND UPPER(lastname) = 'ROSSO';</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A57" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B57" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="C57" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="D57" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='joaosomar13@gmail.com', phone_number='+41766936814' WHERE UPPER(firstname) = 'JOAO' AND UPPER(lastname) = 'RAMOS';</v>
+        <v>UPDATE users SET email='schindlerrene@yahoo.fr', phone_number='+41788636364' WHERE UPPER(firstname) = 'RENÉ' AND UPPER(lastname) = 'SCHINDLER';</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A58" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B58" t="s">
-        <v>219</v>
+        <v>52</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D58" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='martine_robyr@hotmail.com', phone_number='+41765687392' WHERE UPPER(firstname) = 'MARTINE' AND UPPER(lastname) = 'ROBYR';</v>
+        <v>UPDATE users SET email='pschu13@gmail.com', phone_number='+41799067254' WHERE UPPER(firstname) = 'PAUL' AND UPPER(lastname) = 'SCHUMACHER';</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
+        <v>215</v>
+      </c>
+      <c r="B59" t="s">
+        <v>216</v>
+      </c>
+      <c r="C59" t="s">
+        <v>217</v>
+      </c>
+      <c r="D59" t="s">
         <v>218</v>
       </c>
-      <c r="B59" t="s">
-        <v>222</v>
-      </c>
-      <c r="C59" t="s">
-        <v>223</v>
-      </c>
-      <c r="D59" t="s">
-        <v>224</v>
-      </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='robyrs@bluewin.ch', phone_number='+41794248620' WHERE UPPER(firstname) = 'STÉPHANIE' AND UPPER(lastname) = 'ROBYR';</v>
+        <v>UPDATE users SET email='claudiostighezza@hotmail.com', phone_number='+41792206874' WHERE UPPER(firstname) = 'CLAUDIO' AND UPPER(lastname) = 'STIGHEZZA';</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A60" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="B60" t="s">
-        <v>226</v>
+        <v>36</v>
       </c>
       <c r="C60" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="D60" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='troch@windowslive.com', phone_number='+41796587802' WHERE UPPER(firstname) = 'THIERRY' AND UPPER(lastname) = 'ROCH';</v>
+        <v>UPDATE users SET email='julientappy@me.com', phone_number='+41792137876' WHERE UPPER(firstname) = 'JULIEN' AND UPPER(lastname) = 'TAPPY';</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A61" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B61" t="s">
-        <v>65</v>
+        <v>223</v>
       </c>
       <c r="C61" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="D61" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>UPDATE users SET email='marcrosso@hotmail.com', phone_number='+41786770997' WHERE UPPER(firstname) = 'MARC' AND UPPER(lastname) = 'ROSSO';</v>
+        <v>UPDATE users SET email='laura_ujvari@msn.com', phone_number='+41786705977' WHERE UPPER(firstname) = 'LAURA' AND UPPER(lastname) = 'UJVARI';</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A62" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="B62" t="s">
-        <v>233</v>
+        <v>36</v>
       </c>
       <c r="C62" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="F62" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE users SET email='schindlerrene@yahoo.fr', phone_number='+41788636364' WHERE UPPER(firstname) = 'RENÉ' AND UPPER(lastname) = 'SCHINDLER';</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A63" t="s">
-        <v>236</v>
-      </c>
-      <c r="B63" t="s">
-        <v>53</v>
-      </c>
-      <c r="C63" t="s">
-        <v>237</v>
-      </c>
-      <c r="D63" t="s">
-        <v>238</v>
-      </c>
-      <c r="F63" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE users SET email='pschu13@gmail.com', phone_number='+41799067254' WHERE UPPER(firstname) = 'PAUL' AND UPPER(lastname) = 'SCHUMACHER';</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A64" t="s">
-        <v>239</v>
-      </c>
-      <c r="B64" t="s">
-        <v>240</v>
-      </c>
-      <c r="C64" t="s">
-        <v>241</v>
-      </c>
-      <c r="D64" t="s">
-        <v>242</v>
-      </c>
-      <c r="F64" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE users SET email='claudiostighezza@hotmail.com', phone_number='+41792206874' WHERE UPPER(firstname) = 'CLAUDIO' AND UPPER(lastname) = 'STIGHEZZA';</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>243</v>
-      </c>
-      <c r="B65" t="s">
-        <v>37</v>
-      </c>
-      <c r="C65" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" t="s">
-        <v>245</v>
-      </c>
-      <c r="F65" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE users SET email='julientappy@me.com', phone_number='+41792137876' WHERE UPPER(firstname) = 'JULIEN' AND UPPER(lastname) = 'TAPPY';</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>246</v>
-      </c>
-      <c r="B66" t="s">
-        <v>247</v>
-      </c>
-      <c r="C66" t="s">
-        <v>248</v>
-      </c>
-      <c r="D66" t="s">
-        <v>249</v>
-      </c>
-      <c r="F66" t="str">
-        <f t="shared" si="0"/>
-        <v>UPDATE users SET email='laura_ujvari@msn.com', phone_number='+41786705977' WHERE UPPER(firstname) = 'LAURA' AND UPPER(lastname) = 'UJVARI';</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>250</v>
-      </c>
-      <c r="B67" t="s">
-        <v>37</v>
-      </c>
-      <c r="C67" t="s">
-        <v>251</v>
-      </c>
-      <c r="D67" t="s">
-        <v>252</v>
-      </c>
-      <c r="F67" t="str">
-        <f t="shared" ref="F67" si="1">"UPDATE users SET email='" &amp;C67 &amp; "', phone_number='" &amp; D67 &amp; "' WHERE UPPER(firstname) = '" &amp; UPPER(B67) &amp; "' AND UPPER(lastname) = '" &amp; UPPER(A67) &amp; "';"</f>
+        <f t="shared" ref="F62" si="1">"UPDATE users SET email='" &amp;C62 &amp; "', phone_number='" &amp; D62 &amp; "' WHERE UPPER(firstname) = '" &amp; UPPER(B62) &amp; "' AND UPPER(lastname) = '" &amp; UPPER(A62) &amp; "';"</f>
         <v>UPDATE users SET email='julien.wolf@sportsevents.ch', phone_number='+41786966890' WHERE UPPER(firstname) = 'JULIEN' AND UPPER(lastname) = 'WOLF';</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D67"/>
+  <autoFilter ref="A1:D62"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0"/>
 </worksheet>

</xml_diff>